<commit_message>
Create Account Test Added
Create Account using Excel
Account verification
</commit_message>
<xml_diff>
--- a/data/LocationSampleData.xlsx
+++ b/data/LocationSampleData.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{3B13F315-1C21-4DA5-94FE-3B192D0A08B6}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2A36BD-4AD7-4741-86A4-FDB18E875A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView tabRatio="773" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BasicInfo" r:id="rId1" sheetId="1"/>
-    <sheet name="BusinessInfo" r:id="rId2" sheetId="2"/>
-    <sheet name="Products" r:id="rId3" sheetId="3"/>
-    <sheet name="SiteSpecificInfo" r:id="rId4" sheetId="5"/>
-    <sheet name="UpdateOptions" r:id="rId5" sheetId="4"/>
-    <sheet name="LocationUpdates" r:id="rId6" sheetId="6"/>
-    <sheet name="All vendors List" r:id="rId7" sheetId="7"/>
+    <sheet name="BasicInfo" sheetId="1" r:id="rId1"/>
+    <sheet name="BusinessInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="Products" sheetId="3" r:id="rId3"/>
+    <sheet name="SiteSpecificInfo" sheetId="5" r:id="rId4"/>
+    <sheet name="UpdateOptions" sheetId="4" r:id="rId5"/>
+    <sheet name="LocationUpdates" sheetId="6" r:id="rId6"/>
+    <sheet name="All vendors List" sheetId="7" r:id="rId7"/>
+    <sheet name="AccountInfo" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="111">
   <si>
     <t xml:space="preserve">ReferenceCode </t>
   </si>
@@ -169,129 +170,203 @@
     <t>English - Canada</t>
   </si>
   <si>
+    <t>DTC_Type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Location Number</t>
+  </si>
+  <si>
+    <t>Current Status</t>
+  </si>
+  <si>
+    <t>Vendor Id</t>
+  </si>
+  <si>
+    <t>RE-ACTIVATED</t>
+  </si>
+  <si>
+    <t>9990418954</t>
+  </si>
+  <si>
+    <t>DEACTIVATED</t>
+  </si>
+  <si>
+    <t>Factual</t>
+  </si>
+  <si>
+    <t>Brownbook</t>
+  </si>
+  <si>
+    <t>Clinia</t>
+  </si>
+  <si>
+    <t>Cylex</t>
+  </si>
+  <si>
+    <t>Industry Canada</t>
+  </si>
+  <si>
+    <t>Infogroup</t>
+  </si>
+  <si>
+    <t>TomTom</t>
+  </si>
+  <si>
+    <t>TripAdvisor</t>
+  </si>
+  <si>
+    <t>9000199076</t>
+  </si>
+  <si>
+    <t>RE-OPEN</t>
+  </si>
+  <si>
+    <t>DELETED</t>
+  </si>
+  <si>
+    <t>CLOSED</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>LocationName</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>6135550141</t>
+  </si>
+  <si>
+    <t>205 Sherway Gardens Rd</t>
+  </si>
+  <si>
+    <t>M9C 0A5</t>
+  </si>
+  <si>
+    <t>Abi test</t>
+  </si>
+  <si>
     <t>NEW</t>
   </si>
   <si>
-    <t>DTC_Type</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Location Number</t>
-  </si>
-  <si>
-    <t>Current Status</t>
-  </si>
-  <si>
-    <t>Vendor Id</t>
-  </si>
-  <si>
-    <t>RE-ACTIVATED</t>
-  </si>
-  <si>
-    <t>9990418954</t>
-  </si>
-  <si>
-    <t>DEACTIVATED</t>
-  </si>
-  <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>Quebec</t>
-  </si>
-  <si>
-    <t>Factual</t>
-  </si>
-  <si>
-    <t>Brownbook</t>
-  </si>
-  <si>
-    <t>Clinia</t>
-  </si>
-  <si>
-    <t>Cylex</t>
-  </si>
-  <si>
-    <t>Industry Canada</t>
-  </si>
-  <si>
-    <t>Infogroup</t>
-  </si>
-  <si>
-    <t>TomTom</t>
-  </si>
-  <si>
-    <t>TripAdvisor</t>
-  </si>
-  <si>
-    <t>GS Inspection</t>
-  </si>
-  <si>
-    <t>204 Rue des Cèdres</t>
-  </si>
-  <si>
-    <t>Saint-Eustache</t>
-  </si>
-  <si>
-    <t>J7R 2M6</t>
-  </si>
-  <si>
-    <t>6135550333</t>
-  </si>
-  <si>
-    <t>9000199076</t>
-  </si>
-  <si>
-    <t>RE-OPEN</t>
-  </si>
-  <si>
-    <t>DELETED</t>
-  </si>
-  <si>
-    <t>CLOSED</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>LocationName</t>
-  </si>
-  <si>
-    <t>SA Test DRS</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>9000226735</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>9000226737</t>
-  </si>
-  <si>
-    <t>9000226738</t>
-  </si>
-  <si>
-    <t>9000226739</t>
-  </si>
-  <si>
-    <t>GS Inspection1590769532512</t>
+    <t>Aurify Brands Test Account - DTC</t>
+  </si>
+  <si>
+    <t>9000226876</t>
+  </si>
+  <si>
+    <t>Abi test1591707464381</t>
+  </si>
+  <si>
+    <t>9000226877</t>
+  </si>
+  <si>
+    <t>Abi test1591707585892</t>
+  </si>
+  <si>
+    <t>9000226878</t>
+  </si>
+  <si>
+    <t>Abi test1591707695728</t>
+  </si>
+  <si>
+    <t>9000226879</t>
+  </si>
+  <si>
+    <t>Abi test1591707803505</t>
+  </si>
+  <si>
+    <t>9000226880</t>
+  </si>
+  <si>
+    <t>Abi test1591707909970</t>
+  </si>
+  <si>
+    <t>OSAName</t>
+  </si>
+  <si>
+    <t>OSAEmail</t>
+  </si>
+  <si>
+    <t>BusinessUnit</t>
+  </si>
+  <si>
+    <t>ParentAccount</t>
+  </si>
+  <si>
+    <t>MappingAccount</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Sajith DR</t>
+  </si>
+  <si>
+    <t>cseetestreseller@gmail.com</t>
+  </si>
+  <si>
+    <t>IN India</t>
+  </si>
+  <si>
+    <t>34/1000 Old NH 47</t>
+  </si>
+  <si>
+    <t>Edappally Junction</t>
+  </si>
+  <si>
+    <t>Nethaji Nagar</t>
+  </si>
+  <si>
+    <t>Edappally</t>
+  </si>
+  <si>
+    <t>Kochi</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>682024</t>
+  </si>
+  <si>
+    <t>9847713003</t>
+  </si>
+  <si>
+    <t>www.test.com</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>AccountName_Sample</t>
+  </si>
+  <si>
+    <t>Automation_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +379,14 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -323,19 +406,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -352,10 +438,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -390,7 +476,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -425,7 +511,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -519,21 +605,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -550,7 +636,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -602,38 +688,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="10" max="11" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -692,73 +778,242 @@
         <v>35</v>
       </c>
       <c r="S1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="T1" t="s">
         <v>36</v>
       </c>
       <c r="U1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q2" t="s">
         <v>46</v>
       </c>
       <c r="R2" t="s">
+        <v>77</v>
+      </c>
+      <c r="S2" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" t="s">
+        <v>79</v>
+      </c>
+      <c r="S3" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4" t="s">
+        <v>82</v>
+      </c>
+      <c r="T4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" t="s">
+        <v>83</v>
+      </c>
+      <c r="S5" t="s">
         <v>84</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" t="s">
         <v>85</v>
       </c>
-      <c r="T2" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" t="s">
-        <v>56</v>
+      <c r="S6" t="s">
+        <v>86</v>
+      </c>
+      <c r="T6" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F50877-EBD2-44DD-9446-1CDEDBB35701}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F50877-EBD2-44DD-9446-1CDEDBB35701}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -766,9 +1021,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,23 +1049,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A9712B-8B13-418B-BF5E-95B638AECF3E}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A9712B-8B13-418B-BF5E-95B638AECF3E}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -821,50 +1076,25 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -872,8 +1102,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -893,13 +1123,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B8"/>
@@ -972,88 +1202,88 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1069,7 +1299,7 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1077,12 +1307,12 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -1090,7 +1320,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>3628</v>
@@ -1098,7 +1328,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -1114,7 +1344,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -1132,8 +1362,8 @@
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10">
-        <v>1</v>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1146,7 +1376,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>15</v>
@@ -1154,7 +1384,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1162,7 +1392,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -1170,7 +1400,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B15">
         <v>18</v>
@@ -1185,6 +1415,158 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B18A5-D2CF-4D72-983F-92450B03E646}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>92</v>
+      </c>
+      <c r="T1" t="s">
+        <v>93</v>
+      </c>
+      <c r="U1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{C832D280-B991-40FD-ABE4-4187C288BCE8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Create Location with vendors in "Basic info" tab
added a new column for accommodate vendor id and name
</commit_message>
<xml_diff>
--- a/data/LocationSampleData.xlsx
+++ b/data/LocationSampleData.xlsx
@@ -3,19 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2A36BD-4AD7-4741-86A4-FDB18E875A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC69B646-5C7F-4627-ACD4-2862EE942077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicInfo" sheetId="1" r:id="rId1"/>
     <sheet name="BusinessInfo" sheetId="2" r:id="rId2"/>
-    <sheet name="Products" sheetId="3" r:id="rId3"/>
-    <sheet name="SiteSpecificInfo" sheetId="5" r:id="rId4"/>
-    <sheet name="UpdateOptions" sheetId="4" r:id="rId5"/>
-    <sheet name="LocationUpdates" sheetId="6" r:id="rId6"/>
-    <sheet name="All vendors List" sheetId="7" r:id="rId7"/>
-    <sheet name="AccountInfo" sheetId="8" r:id="rId8"/>
+    <sheet name="SiteSpecificInfo" sheetId="5" r:id="rId3"/>
+    <sheet name="UpdateOptions" sheetId="4" r:id="rId4"/>
+    <sheet name="LocationUpdates" sheetId="6" r:id="rId5"/>
+    <sheet name="All vendors List" sheetId="7" r:id="rId6"/>
+    <sheet name="AccountInfo" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
   <si>
     <t xml:space="preserve">ReferenceCode </t>
   </si>
@@ -77,9 +76,6 @@
     <t>DACCategory</t>
   </si>
   <si>
-    <t>Accountant</t>
-  </si>
-  <si>
     <t>Zipcode</t>
   </si>
   <si>
@@ -170,21 +166,12 @@
     <t>English - Canada</t>
   </si>
   <si>
-    <t>DTC_Type</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Location Number</t>
   </si>
   <si>
     <t>Current Status</t>
   </si>
   <si>
-    <t>Vendor Id</t>
-  </si>
-  <si>
     <t>RE-ACTIVATED</t>
   </si>
   <si>
@@ -251,45 +238,9 @@
     <t>M9C 0A5</t>
   </si>
   <si>
-    <t>Abi test</t>
-  </si>
-  <si>
     <t>NEW</t>
   </si>
   <si>
-    <t>Aurify Brands Test Account - DTC</t>
-  </si>
-  <si>
-    <t>9000226876</t>
-  </si>
-  <si>
-    <t>Abi test1591707464381</t>
-  </si>
-  <si>
-    <t>9000226877</t>
-  </si>
-  <si>
-    <t>Abi test1591707585892</t>
-  </si>
-  <si>
-    <t>9000226878</t>
-  </si>
-  <si>
-    <t>Abi test1591707695728</t>
-  </si>
-  <si>
-    <t>9000226879</t>
-  </si>
-  <si>
-    <t>Abi test1591707803505</t>
-  </si>
-  <si>
-    <t>9000226880</t>
-  </si>
-  <si>
-    <t>Abi test1591707909970</t>
-  </si>
-  <si>
     <t>OSAName</t>
   </si>
   <si>
@@ -360,6 +311,33 @@
   </si>
   <si>
     <t>Automation_</t>
+  </si>
+  <si>
+    <t>SA Test DRS</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Vendors_Create</t>
+  </si>
+  <si>
+    <t>Vendor_Update</t>
+  </si>
+  <si>
+    <t>Vendro_ID_Update</t>
+  </si>
+  <si>
+    <t>Abbey</t>
+  </si>
+  <si>
+    <t>Vendor_ID_Create</t>
+  </si>
+  <si>
+    <t>Google,Bing,Facebook,Zomato</t>
+  </si>
+  <si>
+    <t>1,2,4,29</t>
   </si>
 </sst>
 </file>
@@ -696,15 +674,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -718,11 +696,13 @@
     <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="16.28515625" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -763,10 +743,10 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P1" t="s">
         <v>13</v>
@@ -775,234 +755,68 @@
         <v>14</v>
       </c>
       <c r="R1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U1" t="s">
+        <v>99</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
+        <v>102</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X2" t="s">
         <v>70</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" t="s">
-        <v>77</v>
-      </c>
-      <c r="S2" t="s">
-        <v>78</v>
-      </c>
-      <c r="T2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M3" t="s">
-        <v>69</v>
-      </c>
-      <c r="N3" t="s">
-        <v>70</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" t="s">
-        <v>79</v>
-      </c>
-      <c r="S3" t="s">
-        <v>80</v>
-      </c>
-      <c r="T3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M4" t="s">
-        <v>69</v>
-      </c>
-      <c r="N4" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>46</v>
-      </c>
-      <c r="R4" t="s">
-        <v>81</v>
-      </c>
-      <c r="S4" t="s">
-        <v>82</v>
-      </c>
-      <c r="T4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>72</v>
-      </c>
-      <c r="M5" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" t="s">
-        <v>70</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>46</v>
-      </c>
-      <c r="R5" t="s">
-        <v>83</v>
-      </c>
-      <c r="S5" t="s">
-        <v>84</v>
-      </c>
-      <c r="T5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
-      <c r="M6" t="s">
-        <v>69</v>
-      </c>
-      <c r="N6" t="s">
-        <v>70</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>46</v>
-      </c>
-      <c r="R6" t="s">
-        <v>85</v>
-      </c>
-      <c r="S6" t="s">
-        <v>86</v>
-      </c>
-      <c r="T6" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1016,7 +830,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,21 +845,21 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1055,49 +869,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A9712B-8B13-418B-BF5E-95B638AECF3E}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,18 +884,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1139,66 +915,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1222,50 +998,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1273,12 +1049,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,15 +1064,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -1304,7 +1080,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1312,7 +1088,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -1320,7 +1096,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>3628</v>
@@ -1328,7 +1104,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -1336,7 +1112,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1344,7 +1120,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -1352,7 +1128,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1360,15 +1136,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1376,7 +1152,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>15</v>
@@ -1384,7 +1160,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1392,7 +1168,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -1400,7 +1176,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <v>18</v>
@@ -1408,7 +1184,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>29</v>
@@ -1419,12 +1195,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B18A5-D2CF-4D72-983F-92450B03E646}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,25 +1226,25 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1495,72 +1271,72 @@
         <v>12</v>
       </c>
       <c r="P1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
         <v>13</v>
       </c>
       <c r="S1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="T1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="U1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="N2" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="O2" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="P2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test data file
</commit_message>
<xml_diff>
--- a/data/LocationSampleData.xlsx
+++ b/data/LocationSampleData.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{99AA0078-86A9-46CC-85E6-D5CC888F5BCD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6C7471-B83C-4DEC-AE61-1B4F6F438D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" tabRatio="773" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="9"/>
-    <sheet name="AccountInfo" r:id="rId2" sheetId="8"/>
-    <sheet name="BasicInfo" r:id="rId3" sheetId="1"/>
-    <sheet name="BusinessInfo" r:id="rId4" sheetId="2"/>
-    <sheet name="SiteSpecificInfo" r:id="rId5" sheetId="5"/>
-    <sheet name="UpdateOptions" r:id="rId6" sheetId="4"/>
-    <sheet name="LocationUpdates" r:id="rId7" sheetId="6"/>
-    <sheet name="All vendors List" r:id="rId8" sheetId="7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
+    <sheet name="AccountInfo" sheetId="8" r:id="rId2"/>
+    <sheet name="BasicInfo" sheetId="1" r:id="rId3"/>
+    <sheet name="BusinessInfo" sheetId="2" r:id="rId4"/>
+    <sheet name="SiteSpecificInfo" sheetId="5" r:id="rId5"/>
+    <sheet name="UpdateOptions" sheetId="4" r:id="rId6"/>
+    <sheet name="LocationUpdates" sheetId="6" r:id="rId7"/>
+    <sheet name="All vendors List" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="152">
   <si>
     <t>LO_number</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Test House API</t>
   </si>
   <si>
-    <t>Bing,Foursquare</t>
-  </si>
-  <si>
     <t>Test House API1594996456942</t>
   </si>
   <si>
@@ -454,30 +451,53 @@
     <t>Status Text</t>
   </si>
   <si>
-    <t>Apple,Bing,Facebook,Factual,Foursquare,HERE,TomTom,TripAdvisor,Zomato</t>
-  </si>
-  <si>
-    <t>9990308856</t>
-  </si>
-  <si>
     <t>In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress</t>
   </si>
   <si>
     <t>Submitted,Submitted,Submitted,Submitted,Submitted,Submitted,Submitted,Submitted,Submitted</t>
   </si>
   <si>
-    <t>Apple,HERE,TomTom,Zomato</t>
-  </si>
-  <si>
-    <t>In Progress,In Progress,In Progress,In Progress</t>
+    <t>LPAD_Status</t>
+  </si>
+  <si>
+    <t>Submitted,Submitted,Submitted,Submitted,Submitted</t>
+  </si>
+  <si>
+    <t>Apple,Bing,Facebook,Factual,Foursquare,Google,HERE,Tom Tom,Trip Advisor,Zomato</t>
+  </si>
+  <si>
+    <t>Bing,Google,Foursquare</t>
+  </si>
+  <si>
+    <t>9000230201</t>
+  </si>
+  <si>
+    <t>9000230202</t>
+  </si>
+  <si>
+    <t>9000230203</t>
+  </si>
+  <si>
+    <t>9000230204</t>
+  </si>
+  <si>
+    <t>9000230205</t>
+  </si>
+  <si>
+    <t>Submitted,Submitted,Submitted</t>
+  </si>
+  <si>
+    <t>In Progress,In Progress,In Progress</t>
+  </si>
+  <si>
+    <t>Apple,Bing,HERE,Tom Tom,Zomato</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,6 +534,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF797979"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -555,27 +580,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="4" numFmtId="0" quotePrefix="1" xfId="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -592,10 +618,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -630,7 +656,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -665,7 +691,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -759,21 +785,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -790,7 +816,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -842,15 +868,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD27966-DB84-4514-AF6D-7FE75B5D42B0}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD27966-DB84-4514-AF6D-7FE75B5D42B0}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A5"/>
@@ -858,15 +884,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -883,7 +909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -901,7 +927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="15.75" r="3" spans="1:6" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -917,13 +943,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B18A5-D2CF-4D72-983F-92450B03E646}">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B18A5-D2CF-4D72-983F-92450B03E646}">
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -931,23 +957,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="10" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="12" max="13" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="20" max="21" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -1067,47 +1093,48 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S2" xr:uid="{C832D280-B991-40FD-ABE4-4187C288BCE8}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{C832D280-B991-40FD-ABE4-4187C288BCE8}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="10" max="11" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="54.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="103.85546875" collapsed="true"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="54.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="103.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="96" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1184,10 +1211,13 @@
         <v>61</v>
       </c>
       <c r="Z1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
@@ -1221,13 +1251,13 @@
         <v>70</v>
       </c>
       <c r="R2" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>140</v>
+      <c r="V2" t="s">
+        <v>144</v>
       </c>
       <c r="W2" t="s">
         <v>72</v>
@@ -1241,8 +1271,11 @@
       <c r="Z2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>62</v>
       </c>
@@ -1274,13 +1307,13 @@
         <v>70</v>
       </c>
       <c r="R3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>140</v>
+      <c r="V3" t="s">
+        <v>145</v>
       </c>
       <c r="W3" t="s">
         <v>79</v>
@@ -1292,10 +1325,13 @@
         <v>80</v>
       </c>
       <c r="Z3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>62</v>
       </c>
@@ -1327,13 +1363,13 @@
         <v>70</v>
       </c>
       <c r="R4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>140</v>
+      <c r="V4" t="s">
+        <v>146</v>
       </c>
       <c r="W4" t="s">
         <v>83</v>
@@ -1345,10 +1381,13 @@
         <v>84</v>
       </c>
       <c r="Z4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>62</v>
       </c>
@@ -1380,13 +1419,13 @@
         <v>70</v>
       </c>
       <c r="R5" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>140</v>
+      <c r="V5" t="s">
+        <v>147</v>
       </c>
       <c r="W5" t="s">
         <v>88</v>
@@ -1398,10 +1437,13 @@
         <v>89</v>
       </c>
       <c r="Z5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>90</v>
       </c>
@@ -1432,37 +1474,40 @@
       <c r="Q6" t="s">
         <v>70</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="8" t="s">
         <v>143</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>140</v>
+      <c r="V6" t="s">
+        <v>148</v>
       </c>
       <c r="W6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X6" t="s">
         <v>73</v>
       </c>
       <c r="Y6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z6" t="s">
-        <v>144</v>
+        <v>149</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F50877-EBD2-44DD-9446-1CDEDBB35701}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F50877-EBD2-44DD-9446-1CDEDBB35701}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1470,42 +1515,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>96</v>
-      </c>
-      <c r="C1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A1:B2"/>
@@ -1513,34 +1558,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
         <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1550,76 +1595,76 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>120</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
@@ -1627,66 +1672,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
         <v>121</v>
-      </c>
-      <c r="B1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
         <v>123</v>
-      </c>
-      <c r="B2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
         <v>125</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
         <v>127</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -1694,20 +1739,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -1715,7 +1760,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1723,7 +1768,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -1731,7 +1776,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5">
         <v>3628</v>
@@ -1739,7 +1784,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -1747,7 +1792,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1763,7 +1808,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1771,15 +1816,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1787,7 +1832,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12">
         <v>15</v>
@@ -1795,7 +1840,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1803,7 +1848,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -1811,7 +1856,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15">
         <v>18</v>
@@ -1819,13 +1864,13 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for Created location
with Details tab - Social info URL's

Apple Amenities

Added new fields in Business Info Tab
</commit_message>
<xml_diff>
--- a/data/LocationSampleData.xlsx
+++ b/data/LocationSampleData.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC69B646-5C7F-4627-ACD4-2862EE942077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{85959F90-EBCB-42B8-A189-367612066C94}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView tabRatio="773" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="BasicInfo" sheetId="1" r:id="rId1"/>
-    <sheet name="BusinessInfo" sheetId="2" r:id="rId2"/>
-    <sheet name="SiteSpecificInfo" sheetId="5" r:id="rId3"/>
-    <sheet name="UpdateOptions" sheetId="4" r:id="rId4"/>
-    <sheet name="LocationUpdates" sheetId="6" r:id="rId5"/>
-    <sheet name="All vendors List" sheetId="7" r:id="rId6"/>
-    <sheet name="AccountInfo" sheetId="8" r:id="rId7"/>
+    <sheet name="BasicInfo" r:id="rId1" sheetId="1"/>
+    <sheet name="BusinessInfo" r:id="rId2" sheetId="2"/>
+    <sheet name="SiteSpecificInfo" r:id="rId3" sheetId="5"/>
+    <sheet name="Details" r:id="rId4" sheetId="9"/>
+    <sheet name="UpdateOptions" r:id="rId5" sheetId="4"/>
+    <sheet name="LocationUpdates" r:id="rId6" sheetId="6"/>
+    <sheet name="All vendors List" r:id="rId7" sheetId="7"/>
+    <sheet name="AccountInfo" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="158">
   <si>
     <t xml:space="preserve">ReferenceCode </t>
   </si>
@@ -238,112 +239,275 @@
     <t>M9C 0A5</t>
   </si>
   <si>
+    <t>OSAName</t>
+  </si>
+  <si>
+    <t>OSAEmail</t>
+  </si>
+  <si>
+    <t>BusinessUnit</t>
+  </si>
+  <si>
+    <t>ParentAccount</t>
+  </si>
+  <si>
+    <t>MappingAccount</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Sajith DR</t>
+  </si>
+  <si>
+    <t>cseetestreseller@gmail.com</t>
+  </si>
+  <si>
+    <t>IN India</t>
+  </si>
+  <si>
+    <t>34/1000 Old NH 47</t>
+  </si>
+  <si>
+    <t>Edappally Junction</t>
+  </si>
+  <si>
+    <t>Nethaji Nagar</t>
+  </si>
+  <si>
+    <t>Edappally</t>
+  </si>
+  <si>
+    <t>Kochi</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>682024</t>
+  </si>
+  <si>
+    <t>9847713003</t>
+  </si>
+  <si>
+    <t>www.test.com</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>AccountName_Sample</t>
+  </si>
+  <si>
+    <t>Automation_</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Vendors_Create</t>
+  </si>
+  <si>
+    <t>Vendor_Update</t>
+  </si>
+  <si>
+    <t>Vendro_ID_Update</t>
+  </si>
+  <si>
+    <t>Abbey</t>
+  </si>
+  <si>
+    <t>Vendor_ID_Create</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>FaxNumber</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>TollFreeNumber</t>
+  </si>
+  <si>
+    <t>LandLineNumber</t>
+  </si>
+  <si>
+    <t>BusinessWebsite</t>
+  </si>
+  <si>
+    <t>AppleBusinessName</t>
+  </si>
+  <si>
+    <t>AppleAmenites</t>
+  </si>
+  <si>
+    <t>Video_URL</t>
+  </si>
+  <si>
+    <t>LinkedIn_URL</t>
+  </si>
+  <si>
+    <t>Twitter_URL</t>
+  </si>
+  <si>
+    <t>Facebook_URL</t>
+  </si>
+  <si>
+    <t>Test Apple name</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>18003243198</t>
+  </si>
+  <si>
+    <t>Transmission and status</t>
+  </si>
+  <si>
+    <t>American Express,Apple Pay</t>
+  </si>
+  <si>
+    <t>Delivery, 24-Hour Front Desk</t>
+  </si>
+  <si>
+    <t>CSEE_Test Account_Sajith</t>
+  </si>
+  <si>
+    <t>0001000</t>
+  </si>
+  <si>
+    <t>0001001</t>
+  </si>
+  <si>
+    <t>Apple,Google,Bing,Facebook</t>
+  </si>
+  <si>
+    <t>1,20,2,4</t>
+  </si>
+  <si>
     <t>NEW</t>
   </si>
   <si>
-    <t>OSAName</t>
-  </si>
-  <si>
-    <t>OSAEmail</t>
-  </si>
-  <si>
-    <t>BusinessUnit</t>
-  </si>
-  <si>
-    <t>ParentAccount</t>
-  </si>
-  <si>
-    <t>MappingAccount</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>StartDate</t>
-  </si>
-  <si>
-    <t>EndDate</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Sajith DR</t>
-  </si>
-  <si>
-    <t>cseetestreseller@gmail.com</t>
-  </si>
-  <si>
-    <t>IN India</t>
-  </si>
-  <si>
-    <t>34/1000 Old NH 47</t>
-  </si>
-  <si>
-    <t>Edappally Junction</t>
-  </si>
-  <si>
-    <t>Nethaji Nagar</t>
-  </si>
-  <si>
-    <t>Edappally</t>
-  </si>
-  <si>
-    <t>Kochi</t>
-  </si>
-  <si>
-    <t>Kerala</t>
-  </si>
-  <si>
-    <t>682024</t>
-  </si>
-  <si>
-    <t>9847713003</t>
-  </si>
-  <si>
-    <t>www.test.com</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>AccountName_Sample</t>
-  </si>
-  <si>
-    <t>Automation_</t>
-  </si>
-  <si>
-    <t>SA Test DRS</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Vendors_Create</t>
-  </si>
-  <si>
-    <t>Vendor_Update</t>
-  </si>
-  <si>
-    <t>Vendro_ID_Update</t>
-  </si>
-  <si>
-    <t>Abbey</t>
-  </si>
-  <si>
-    <t>Vendor_ID_Create</t>
+    <t>www.facebook.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.twitter.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.video.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.pinterest.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.instagram.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.social.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.coupon.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.menu.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.reservations.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.order.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.appointment.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.inventory.com/testautomation</t>
+  </si>
+  <si>
+    <t>www.virtualcare.com/testautomation</t>
+  </si>
+  <si>
+    <t>Pinterest_URL</t>
+  </si>
+  <si>
+    <t>Instagram_URL</t>
+  </si>
+  <si>
+    <t>VirtualCare_URL</t>
+  </si>
+  <si>
+    <t>InventorySearch_URL</t>
+  </si>
+  <si>
+    <t>Appointment_URL</t>
+  </si>
+  <si>
+    <t>OrderAhead_URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reservations_URL </t>
+  </si>
+  <si>
+    <t>Menu_URL</t>
+  </si>
+  <si>
+    <t>Coupon_URL</t>
+  </si>
+  <si>
+    <t>SocialNetwork_URL</t>
   </si>
   <si>
     <t>Google,Bing,Facebook,Zomato</t>
   </si>
   <si>
     <t>1,2,4,29</t>
+  </si>
+  <si>
+    <t>9000230515</t>
+  </si>
+  <si>
+    <t>Automation1597422810498</t>
+  </si>
+  <si>
+    <t>43.609272</t>
+  </si>
+  <si>
+    <t>-79.557008</t>
+  </si>
+  <si>
+    <t>9000230516</t>
+  </si>
+  <si>
+    <t>Automation1597423023246</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,21 +549,21 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -416,10 +580,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -454,7 +618,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -489,7 +653,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -583,21 +747,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -614,7 +778,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -666,43 +830,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="16.28515625" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="8" max="9" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="10" max="11" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="34.7109375" collapsed="false"/>
+    <col min="19" max="21" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="22.42578125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -755,16 +920,16 @@
         <v>14</v>
       </c>
       <c r="R1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" t="s">
+        <v>96</v>
+      </c>
+      <c r="U1" t="s">
         <v>97</v>
-      </c>
-      <c r="S1" t="s">
-        <v>101</v>
-      </c>
-      <c r="T1" t="s">
-        <v>98</v>
-      </c>
-      <c r="U1" t="s">
-        <v>99</v>
       </c>
       <c r="V1" t="s">
         <v>34</v>
@@ -773,20 +938,31 @@
         <v>64</v>
       </c>
       <c r="X1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
@@ -794,6 +970,9 @@
       <c r="G2" t="s">
         <v>68</v>
       </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
       <c r="M2" t="s">
         <v>65</v>
       </c>
@@ -810,37 +989,123 @@
         <v>45</v>
       </c>
       <c r="R2" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>103</v>
+        <v>151</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V2" t="s">
+        <v>152</v>
+      </c>
+      <c r="W2" t="s">
+        <v>153</v>
       </c>
       <c r="X2" t="s">
-        <v>70</v>
+        <v>154</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" t="s">
+        <v>123</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V3" t="s">
+        <v>156</v>
+      </c>
+      <c r="W3" t="s">
+        <v>157</v>
+      </c>
+      <c r="X3" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F50877-EBD2-44DD-9446-1CDEDBB35701}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F50877-EBD2-44DD-9446-1CDEDBB35701}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="4" max="8" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="27.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -850,10 +1115,28 @@
       <c r="C1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -861,51 +1144,209 @@
       <c r="C2" t="s">
         <v>39</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="H2" xr:uid="{1905EB81-0F12-4F11-AE51-666D49C35ECD}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:B2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.5703125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AACAE9-1523-469A-9986-B17E432A9632}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="14" bestFit="true" customWidth="true" width="34.140625" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A2" xr:uid="{AD420730-70A7-4316-82A6-856D27566878}"/>
+    <hyperlink r:id="rId2" ref="B2" xr:uid="{D7DC4FD4-F011-4E7F-8AD0-AD1A8C48F1F2}"/>
+    <hyperlink r:id="rId3" ref="C2" xr:uid="{6F106DC6-41EF-4E44-923A-6270375F42A3}"/>
+    <hyperlink r:id="rId4" ref="D2" xr:uid="{548A6CD7-5830-4087-BE07-723B36BFEC5C}"/>
+    <hyperlink r:id="rId5" ref="E2" xr:uid="{20F1DDE7-9E36-491D-AA27-1D3187C246C7}"/>
+    <hyperlink r:id="rId6" ref="F2" xr:uid="{46E35268-AEEE-4DB2-B1DC-98D5E7EB8E38}"/>
+    <hyperlink r:id="rId7" ref="G2" xr:uid="{6AC83006-C804-4663-9B02-3F3A9863B8DC}"/>
+    <hyperlink r:id="rId8" ref="H2" xr:uid="{6CC018D0-461E-4CAA-912F-3495BAB4F14D}"/>
+    <hyperlink r:id="rId9" ref="I2" xr:uid="{81FA1FA2-C7FE-42A7-8234-484F260075D6}"/>
+    <hyperlink r:id="rId10" ref="J2" xr:uid="{0D6003B3-649D-48B1-BBAB-463CD8C52F2A}"/>
+    <hyperlink r:id="rId11" ref="K2" xr:uid="{17033EC0-6910-469D-A9AC-EE3C72276EAB}"/>
+    <hyperlink r:id="rId12" ref="L2" xr:uid="{AB23180B-8E44-40B7-8867-AB42262C48F8}"/>
+    <hyperlink r:id="rId13" ref="M2" xr:uid="{DEB71B11-17C0-4C96-9056-C893C1B13FA3}"/>
+    <hyperlink r:id="rId14" ref="N2" xr:uid="{A53CA81F-80E8-40CF-9D57-D30DD240D7A4}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId15" verticalDpi="4294967295"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B8"/>
@@ -978,13 +1419,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
-  <dimension ref="A1:B6"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
@@ -992,8 +1433,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1045,21 +1486,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
-  <dimension ref="A1:B16"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1191,13 +1632,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B18A5-D2CF-4D72-983F-92450B03E646}">
-  <dimension ref="A1:U2"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B18A5-D2CF-4D72-983F-92450B03E646}">
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
@@ -1205,23 +1646,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="21" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="10" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="12" max="13" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="20" max="21" customWidth="true" width="16.28515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -1229,22 +1670,22 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>74</v>
-      </c>
-      <c r="G1" t="s">
-        <v>75</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1280,69 +1721,69 @@
         <v>13</v>
       </c>
       <c r="S1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" t="s">
         <v>76</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>77</v>
-      </c>
-      <c r="U1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" t="s">
         <v>81</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>82</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>83</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>84</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>85</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>86</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>87</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{C832D280-B991-40FD-ABE4-4187C288BCE8}"/>
+    <hyperlink r:id="rId1" ref="S2" xr:uid="{C832D280-B991-40FD-ABE4-4187C288BCE8}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: LPAD suite integrated with Framework
LAUNCHPAD class dependency removed from pages.


Login test included to Create Location
</commit_message>
<xml_diff>
--- a/data/LocationSampleData.xlsx
+++ b/data/LocationSampleData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{85959F90-EBCB-42B8-A189-367612066C94}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{64EFEAFB-8D16-4DB6-8202-37C2D212412C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView tabRatio="773" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="160">
   <si>
     <t xml:space="preserve">ReferenceCode </t>
   </si>
@@ -485,22 +485,28 @@
     <t>1,2,4,29</t>
   </si>
   <si>
-    <t>9000230515</t>
-  </si>
-  <si>
-    <t>Automation1597422810498</t>
+    <t>9000230592</t>
+  </si>
+  <si>
+    <t>Automation1597929055751</t>
+  </si>
+  <si>
+    <t>43.613122</t>
+  </si>
+  <si>
+    <t>-79.556162</t>
+  </si>
+  <si>
+    <t>9000230593</t>
+  </si>
+  <si>
+    <t>Automation1597929225806</t>
   </si>
   <si>
     <t>43.609272</t>
   </si>
   <si>
     <t>-79.557008</t>
-  </si>
-  <si>
-    <t>9000230516</t>
-  </si>
-  <si>
-    <t>Automation1597423023246</t>
   </si>
 </sst>
 </file>
@@ -841,7 +847,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,10 +1079,10 @@
         <v>157</v>
       </c>
       <c r="X3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="Y3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="Z3" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Manage Location functions Updated
</commit_message>
<xml_diff>
--- a/data/LocationSampleData.xlsx
+++ b/data/LocationSampleData.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{64EFEAFB-8D16-4DB6-8202-37C2D212412C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6934ACF9-01CC-4E8F-9FCC-3746EAA9798C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView tabRatio="773" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BasicInfo" r:id="rId1" sheetId="1"/>
-    <sheet name="BusinessInfo" r:id="rId2" sheetId="2"/>
-    <sheet name="SiteSpecificInfo" r:id="rId3" sheetId="5"/>
-    <sheet name="Details" r:id="rId4" sheetId="9"/>
-    <sheet name="UpdateOptions" r:id="rId5" sheetId="4"/>
-    <sheet name="LocationUpdates" r:id="rId6" sheetId="6"/>
-    <sheet name="All vendors List" r:id="rId7" sheetId="7"/>
-    <sheet name="AccountInfo" r:id="rId8" sheetId="8"/>
+    <sheet name="BasicInfo" sheetId="1" r:id="rId1"/>
+    <sheet name="BusinessInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="SiteSpecificInfo" sheetId="5" r:id="rId3"/>
+    <sheet name="Details" sheetId="9" r:id="rId4"/>
+    <sheet name="UpdateOptions" sheetId="4" r:id="rId5"/>
+    <sheet name="LocationUpdates" sheetId="6" r:id="rId6"/>
+    <sheet name="All vendors List" sheetId="7" r:id="rId7"/>
+    <sheet name="AccountInfo" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="156">
   <si>
     <t xml:space="preserve">ReferenceCode </t>
   </si>
@@ -311,9 +311,6 @@
     <t>Automation_</t>
   </si>
   <si>
-    <t>Automation</t>
-  </si>
-  <si>
     <t>Vendors_Create</t>
   </si>
   <si>
@@ -329,9 +326,6 @@
     <t>Vendor_ID_Create</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -389,21 +383,6 @@
     <t>Delivery, 24-Hour Front Desk</t>
   </si>
   <si>
-    <t>CSEE_Test Account_Sajith</t>
-  </si>
-  <si>
-    <t>0001000</t>
-  </si>
-  <si>
-    <t>0001001</t>
-  </si>
-  <si>
-    <t>Apple,Google,Bing,Facebook</t>
-  </si>
-  <si>
-    <t>1,20,2,4</t>
-  </si>
-  <si>
     <t>NEW</t>
   </si>
   <si>
@@ -479,42 +458,50 @@
     <t>SocialNetwork_URL</t>
   </si>
   <si>
-    <t>Google,Bing,Facebook,Zomato</t>
-  </si>
-  <si>
-    <t>1,2,4,29</t>
-  </si>
-  <si>
-    <t>9000230592</t>
-  </si>
-  <si>
-    <t>Automation1597929055751</t>
-  </si>
-  <si>
-    <t>43.613122</t>
-  </si>
-  <si>
-    <t>-79.556162</t>
-  </si>
-  <si>
-    <t>9000230593</t>
-  </si>
-  <si>
-    <t>Automation1597929225806</t>
-  </si>
-  <si>
-    <t>43.609272</t>
-  </si>
-  <si>
-    <t>-79.557008</t>
+    <t>25082020_1</t>
+  </si>
+  <si>
+    <t>Automation Test</t>
+  </si>
+  <si>
+    <t>Apple,Bing,Facebook,Factual,Foursquare,Google,HERE,Tom Tom,Trip Advisor,Zomato</t>
+  </si>
+  <si>
+    <t>20,2,4,12,3,1,10,30,18,29</t>
+  </si>
+  <si>
+    <t>25082020_2</t>
+  </si>
+  <si>
+    <t>25082020_3</t>
+  </si>
+  <si>
+    <t>25082020_4</t>
+  </si>
+  <si>
+    <t>25082020_5</t>
+  </si>
+  <si>
+    <t>1259 King St W</t>
+  </si>
+  <si>
+    <t>M6K 1G4</t>
+  </si>
+  <si>
+    <t>Bing,Google,Foursquare</t>
+  </si>
+  <si>
+    <t>2,1,3</t>
+  </si>
+  <si>
+    <t>SA Test DRS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,6 +523,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -555,21 +547,22 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -586,10 +579,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -624,7 +617,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -659,7 +652,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -753,21 +746,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -784,7 +777,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -836,41 +829,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="10" max="11" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="34.7109375" collapsed="false"/>
-    <col min="19" max="21" customWidth="true" width="16.28515625" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="22.42578125" collapsed="false"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="34.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -926,16 +920,16 @@
         <v>14</v>
       </c>
       <c r="R1" t="s">
+        <v>94</v>
+      </c>
+      <c r="S1" t="s">
+        <v>98</v>
+      </c>
+      <c r="T1" t="s">
         <v>95</v>
       </c>
-      <c r="S1" t="s">
-        <v>99</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>96</v>
-      </c>
-      <c r="U1" t="s">
-        <v>97</v>
       </c>
       <c r="V1" t="s">
         <v>34</v>
@@ -944,31 +938,31 @@
         <v>64</v>
       </c>
       <c r="X1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Z1" t="s">
         <v>35</v>
       </c>
       <c r="AA1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
@@ -976,9 +970,6 @@
       <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="L2" t="s">
-        <v>66</v>
-      </c>
       <c r="M2" t="s">
         <v>65</v>
       </c>
@@ -995,46 +986,28 @@
         <v>45</v>
       </c>
       <c r="R2" t="s">
-        <v>150</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="V2" t="s">
-        <v>152</v>
-      </c>
-      <c r="W2" t="s">
-        <v>153</v>
-      </c>
-      <c r="X2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>155</v>
+        <v>145</v>
+      </c>
+      <c r="S2" t="s">
+        <v>146</v>
       </c>
       <c r="Z2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
@@ -1042,9 +1015,6 @@
       <c r="G3" t="s">
         <v>68</v>
       </c>
-      <c r="L3" t="s">
-        <v>66</v>
-      </c>
       <c r="M3" t="s">
         <v>65</v>
       </c>
@@ -1061,42 +1031,149 @@
         <v>45</v>
       </c>
       <c r="R3" t="s">
-        <v>123</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="V3" t="s">
-        <v>156</v>
-      </c>
-      <c r="W3" t="s">
-        <v>157</v>
-      </c>
-      <c r="X3" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>159</v>
+        <v>145</v>
+      </c>
+      <c r="S3" t="s">
+        <v>146</v>
       </c>
       <c r="Z3" t="s">
-        <v>125</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" t="s">
+        <v>145</v>
+      </c>
+      <c r="S4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R5" t="s">
+        <v>145</v>
+      </c>
+      <c r="S5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>151</v>
+      </c>
+      <c r="M6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" t="s">
+        <v>152</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F50877-EBD2-44DD-9446-1CDEDBB35701}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F50877-EBD2-44DD-9446-1CDEDBB35701}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -1104,11 +1181,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
-    <col min="4" max="8" customWidth="true" width="16.28515625" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="27.0" collapsed="false"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="8" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1122,27 +1199,27 @@
         <v>37</v>
       </c>
       <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
         <v>103</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>104</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" t="s">
-        <v>107</v>
-      </c>
       <c r="I1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -1157,7 +1234,7 @@
         <v>67</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>67</v>
@@ -1166,21 +1243,21 @@
         <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="H2" xr:uid="{1905EB81-0F12-4F11-AE51-666D49C35ECD}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{1905EB81-0F12-4F11-AE51-666D49C35ECD}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA9752C-CCE4-4407-A606-5597CCC85618}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -1188,10 +1265,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.5703125" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="false"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,10 +1279,10 @@
         <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,20 +1293,20 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AACAE9-1523-469A-9986-B17E432A9632}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AACAE9-1523-469A-9986-B17E432A9632}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
@@ -1237,122 +1314,122 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" bestFit="true" customWidth="true" width="34.140625" collapsed="false"/>
+    <col min="1" max="14" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" t="s">
         <v>140</v>
       </c>
-      <c r="F1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I1" t="s">
-        <v>147</v>
-      </c>
       <c r="J1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="K1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="L1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="M1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="N1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2" xr:uid="{AD420730-70A7-4316-82A6-856D27566878}"/>
-    <hyperlink r:id="rId2" ref="B2" xr:uid="{D7DC4FD4-F011-4E7F-8AD0-AD1A8C48F1F2}"/>
-    <hyperlink r:id="rId3" ref="C2" xr:uid="{6F106DC6-41EF-4E44-923A-6270375F42A3}"/>
-    <hyperlink r:id="rId4" ref="D2" xr:uid="{548A6CD7-5830-4087-BE07-723B36BFEC5C}"/>
-    <hyperlink r:id="rId5" ref="E2" xr:uid="{20F1DDE7-9E36-491D-AA27-1D3187C246C7}"/>
-    <hyperlink r:id="rId6" ref="F2" xr:uid="{46E35268-AEEE-4DB2-B1DC-98D5E7EB8E38}"/>
-    <hyperlink r:id="rId7" ref="G2" xr:uid="{6AC83006-C804-4663-9B02-3F3A9863B8DC}"/>
-    <hyperlink r:id="rId8" ref="H2" xr:uid="{6CC018D0-461E-4CAA-912F-3495BAB4F14D}"/>
-    <hyperlink r:id="rId9" ref="I2" xr:uid="{81FA1FA2-C7FE-42A7-8234-484F260075D6}"/>
-    <hyperlink r:id="rId10" ref="J2" xr:uid="{0D6003B3-649D-48B1-BBAB-463CD8C52F2A}"/>
-    <hyperlink r:id="rId11" ref="K2" xr:uid="{17033EC0-6910-469D-A9AC-EE3C72276EAB}"/>
-    <hyperlink r:id="rId12" ref="L2" xr:uid="{AB23180B-8E44-40B7-8867-AB42262C48F8}"/>
-    <hyperlink r:id="rId13" ref="M2" xr:uid="{DEB71B11-17C0-4C96-9056-C893C1B13FA3}"/>
-    <hyperlink r:id="rId14" ref="N2" xr:uid="{A53CA81F-80E8-40CF-9D57-D30DD240D7A4}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AD420730-70A7-4316-82A6-856D27566878}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{D7DC4FD4-F011-4E7F-8AD0-AD1A8C48F1F2}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{6F106DC6-41EF-4E44-923A-6270375F42A3}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{548A6CD7-5830-4087-BE07-723B36BFEC5C}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{20F1DDE7-9E36-491D-AA27-1D3187C246C7}"/>
+    <hyperlink ref="F2" r:id="rId6" xr:uid="{46E35268-AEEE-4DB2-B1DC-98D5E7EB8E38}"/>
+    <hyperlink ref="G2" r:id="rId7" xr:uid="{6AC83006-C804-4663-9B02-3F3A9863B8DC}"/>
+    <hyperlink ref="H2" r:id="rId8" xr:uid="{6CC018D0-461E-4CAA-912F-3495BAB4F14D}"/>
+    <hyperlink ref="I2" r:id="rId9" xr:uid="{81FA1FA2-C7FE-42A7-8234-484F260075D6}"/>
+    <hyperlink ref="J2" r:id="rId10" xr:uid="{0D6003B3-649D-48B1-BBAB-463CD8C52F2A}"/>
+    <hyperlink ref="K2" r:id="rId11" xr:uid="{17033EC0-6910-469D-A9AC-EE3C72276EAB}"/>
+    <hyperlink ref="L2" r:id="rId12" xr:uid="{AB23180B-8E44-40B7-8867-AB42262C48F8}"/>
+    <hyperlink ref="M2" r:id="rId13" xr:uid="{DEB71B11-17C0-4C96-9056-C893C1B13FA3}"/>
+    <hyperlink ref="N2" r:id="rId14" xr:uid="{A53CA81F-80E8-40CF-9D57-D30DD240D7A4}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId15" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8563A0F8-84BE-4D12-A460-D3604BB1A5E4}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B8"/>
@@ -1425,13 +1502,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DE9A24-7E4D-4E43-805A-982B98AB488A}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
@@ -1439,8 +1516,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1492,13 +1569,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC5FF40-2A06-4382-885C-E53F5AB473FD}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -1506,7 +1583,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1638,37 +1715,37 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B18A5-D2CF-4D72-983F-92450B03E646}">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B18A5-D2CF-4D72-983F-92450B03E646}">
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="10" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="12" max="13" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="20" max="21" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -1788,8 +1865,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S2" xr:uid="{C832D280-B991-40FD-ABE4-4187C288BCE8}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{C832D280-B991-40FD-ABE4-4187C288BCE8}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preset Location Values Update
</commit_message>
<xml_diff>
--- a/data/LocationSampleData.xlsx
+++ b/data/LocationSampleData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7B1604-3361-479C-B101-E0715DABFE78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988D6040-1382-43DB-817F-429E166C72CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
   <si>
     <t xml:space="preserve">ReferenceCode </t>
   </si>
@@ -164,9 +164,6 @@
     <t>CA Canada</t>
   </si>
   <si>
-    <t>English - Canada</t>
-  </si>
-  <si>
     <t>Location Number</t>
   </si>
   <si>
@@ -461,12 +458,6 @@
     <t>Automation Test</t>
   </si>
   <si>
-    <t>Apple,Bing,Facebook,Factual,Foursquare,Google,HERE,Tom Tom,Trip Advisor,Zomato</t>
-  </si>
-  <si>
-    <t>20,2,4,12,3,1,10,30,18,29</t>
-  </si>
-  <si>
     <t>1259 King St W</t>
   </si>
   <si>
@@ -479,25 +470,22 @@
     <t>2,1,3</t>
   </si>
   <si>
-    <t>Aurify Brands - Test</t>
-  </si>
-  <si>
-    <t>Automation Test Account - TSEE</t>
-  </si>
-  <si>
-    <t>25092020_1</t>
-  </si>
-  <si>
-    <t>25092020_2</t>
-  </si>
-  <si>
-    <t>25092020_3</t>
-  </si>
-  <si>
-    <t>25092020_4</t>
-  </si>
-  <si>
-    <t>25092020_5</t>
+    <t>SA Test DRS</t>
+  </si>
+  <si>
+    <t>21062021_1</t>
+  </si>
+  <si>
+    <t>21062021_2</t>
+  </si>
+  <si>
+    <t>English-Canada</t>
+  </si>
+  <si>
+    <t>Apple,Bing,Facebook,Foursquare,Google,HERE,Tom Tom,Trip Advisor,Zomato</t>
+  </si>
+  <si>
+    <t>20,2,4,3,1,10,30,18,29</t>
   </si>
 </sst>
 </file>
@@ -553,13 +541,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -841,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +850,7 @@
     <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="34.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="78.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="21" width="16.28515625" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -924,249 +911,120 @@
         <v>14</v>
       </c>
       <c r="R1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T1" t="s">
         <v>94</v>
       </c>
-      <c r="S1" t="s">
-        <v>98</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>95</v>
-      </c>
-      <c r="U1" t="s">
-        <v>96</v>
       </c>
       <c r="V1" t="s">
         <v>34</v>
       </c>
       <c r="W1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y1" t="s">
         <v>99</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>100</v>
       </c>
       <c r="Z1" t="s">
         <v>35</v>
       </c>
       <c r="AA1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="Q2" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="R2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="S2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="Z2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>149</v>
+      </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="M3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" t="s">
         <v>65</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
+        <v>144</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="Q3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" t="s">
-        <v>144</v>
-      </c>
-      <c r="S3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="Z3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" t="s">
-        <v>65</v>
-      </c>
-      <c r="N4" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>45</v>
-      </c>
-      <c r="R4" t="s">
-        <v>144</v>
-      </c>
-      <c r="S4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" t="s">
-        <v>66</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>45</v>
-      </c>
-      <c r="R5" t="s">
-        <v>144</v>
-      </c>
-      <c r="S5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="S3" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="M6" t="s">
-        <v>65</v>
-      </c>
-      <c r="N6" t="s">
-        <v>66</v>
-      </c>
-      <c r="O6" t="s">
-        <v>147</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1203,27 +1061,27 @@
         <v>37</v>
       </c>
       <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>103</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>104</v>
       </c>
-      <c r="H1" t="s">
-        <v>105</v>
-      </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -1232,22 +1090,22 @@
         <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1283,10 +1141,10 @@
         <v>42</v>
       </c>
       <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
         <v>106</v>
-      </c>
-      <c r="D1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1297,10 +1155,10 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1323,90 +1181,90 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s">
         <v>133</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" t="s">
         <v>134</v>
-      </c>
-      <c r="G1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J1" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" t="s">
-        <v>138</v>
-      </c>
-      <c r="L1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M1" t="s">
-        <v>136</v>
-      </c>
-      <c r="N1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1294,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,50 +1384,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
         <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1616,7 +1474,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -1624,7 +1482,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>3628</v>
@@ -1632,7 +1490,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -1648,7 +1506,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -1680,7 +1538,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12">
         <v>15</v>
@@ -1688,7 +1546,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1696,7 +1554,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -1704,7 +1562,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>18</v>
@@ -1757,22 +1615,22 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>73</v>
-      </c>
-      <c r="G1" t="s">
-        <v>74</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1808,63 +1666,63 @@
         <v>13</v>
       </c>
       <c r="S1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" t="s">
         <v>75</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>76</v>
-      </c>
-      <c r="U1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" t="s">
         <v>80</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>81</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>82</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>83</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>84</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>85</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>86</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>